<commit_message>
* changed variables to match the article
</commit_message>
<xml_diff>
--- a/variable_definitions.xlsx
+++ b/variable_definitions.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -38,67 +38,34 @@
     <t xml:space="preserve">notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ika</t>
+    <t xml:space="preserve">Age (years)</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;missing&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">?,-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heart rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pulse1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?,-,7777</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Systolic blood pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rr1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen saturation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spo21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">777,888,999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time to HEMS arrival</t>
-  </si>
-  <si>
-    <t xml:space="preserve">call_to_patient_min</t>
+    <t xml:space="preserve">Heart rate (bpm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systolic blood pressure (mmHg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxygen saturation (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to HEMS arrival (minutes)</t>
   </si>
   <si>
     <t xml:space="preserve">Glasgow Coma Scale</t>
   </si>
   <si>
-    <t xml:space="preserve">gcst1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sukup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Man</t>
+    <t xml:space="preserve">Patient sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;any other value&gt;</t>
@@ -107,118 +74,61 @@
     <t xml:space="preserve">Cardiac rhythm</t>
   </si>
   <si>
-    <t xml:space="preserve">rhythm1</t>
-  </si>
-  <si>
     <t xml:space="preserve">VF, VT, ASY, PEA</t>
   </si>
   <si>
     <t xml:space="preserve">Other category</t>
   </si>
   <si>
-    <t xml:space="preserve">1,2,3,5,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mission located in a medical facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">med_facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medical facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not medical facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vehicle type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vehicle_type</t>
+    <t xml:space="preserve">Medical facility or nursing home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEMS vehicle</t>
   </si>
   <si>
     <t xml:space="preserve">Ground unit</t>
   </si>
   <si>
-    <t xml:space="preserve">Ground unit,Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Helicopter or BG helicopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BG Helicopter,Helicopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dispatch code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmr</t>
+    <t xml:space="preserve">Helicopter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient group</t>
   </si>
   <si>
     <t xml:space="preserve">Cardiac arrest</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Trauma</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Respiratory failure</t>
   </si>
   <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chest pain</t>
   </si>
   <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Stroke</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Neurological</t>
   </si>
   <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Psychiatric or intoxication</t>
   </si>
   <si>
-    <t xml:space="preserve">7,11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gynecological and obstetrics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
+    <t xml:space="preserve">Gynaecology and obstetrics</t>
   </si>
   <si>
     <t xml:space="preserve">Infection</t>
   </si>
   <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
     <t xml:space="preserve">Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
   </si>
   <si>
     <t xml:space="preserve">column</t>
@@ -407,7 +317,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -441,411 +351,280 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B8" s="5"/>
       <c r="C8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="7" t="n">
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B9" s="5"/>
       <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B10" s="5"/>
       <c r="C10" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B11" s="5"/>
       <c r="C11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="7" t="n">
-        <v>4</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B12" s="5"/>
       <c r="C12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B13" s="5"/>
       <c r="C13" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B14" s="5"/>
       <c r="C14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>35</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B15" s="5"/>
       <c r="C15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B16" s="5"/>
       <c r="C16" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>39</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B17" s="5"/>
       <c r="C17" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>39</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B18" s="5"/>
       <c r="C18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>39</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B19" s="5"/>
       <c r="C19" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>47</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B21" s="5"/>
       <c r="C21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B22" s="5"/>
       <c r="C22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B23" s="5"/>
       <c r="C23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B24" s="5"/>
       <c r="C24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B25" s="5"/>
       <c r="C25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B26" s="5"/>
       <c r="C26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B27" s="5"/>
       <c r="C27" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B28" s="5"/>
       <c r="C28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B29" s="5"/>
       <c r="C29" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B30" s="5"/>
       <c r="C30" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,10 +673,10 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="1" sqref="D50 B27"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="52.24"/>
@@ -906,10 +685,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>4</v>
@@ -920,15 +699,15 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -936,10 +715,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>